<commit_message>
first iteration of spring 2023 checkscripts
</commit_message>
<xml_diff>
--- a/ApRESCalculator.xlsx
+++ b/ApRESCalculator.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/georgelu/Documents/GitHub/processing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31ABDC34-23AB-4443-86EE-EB19257268B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A37D3BFD-1107-1342-8761-23315955E1D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="27160" windowHeight="16200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -151,12 +151,6 @@
     <t>Battery capacity per 6 months (Ahr)</t>
   </si>
   <si>
-    <t>Memory per 3 months (GB)</t>
-  </si>
-  <si>
-    <t>Battery capacity per 3 months (Ahr)</t>
-  </si>
-  <si>
     <t>No Attenuation settings</t>
   </si>
   <si>
@@ -173,6 +167,12 @@
   </si>
   <si>
     <t>Observed memory after 3 months (GB)</t>
+  </si>
+  <si>
+    <t>Memory per 4 months (GB)</t>
+  </si>
+  <si>
+    <t>Battery capacity per 4 months (Ahr)</t>
   </si>
 </sst>
 </file>
@@ -600,7 +600,7 @@
   <dimension ref="A1:J25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="119" zoomScaleNormal="87" workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -643,7 +643,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B5" s="13">
         <v>20</v>
@@ -658,7 +658,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B6" s="13">
         <v>2</v>
@@ -853,11 +853,11 @@
         <v>293.06048583984375</v>
       </c>
       <c r="H19" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="I19">
-        <f>I15/2</f>
-        <v>26.132896106690168</v>
+        <f>F15/3</f>
+        <v>34.843861475586891</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -875,11 +875,11 @@
         <v>0.57107893333333337</v>
       </c>
       <c r="H20" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="I20">
-        <f>I16/2</f>
-        <v>86.911075166666691</v>
+        <f>F16/3</f>
+        <v>69.528860133333339</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.2">
@@ -913,13 +913,13 @@
         <v>12.210853576660156</v>
       </c>
       <c r="H23" s="18" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="I23" s="18">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="J23" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="24" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -937,14 +937,14 @@
         <v>2.3794955555555556E-2</v>
       </c>
       <c r="H24" s="18" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="I24" s="18">
         <f>100*(I23-I19)/I23</f>
-        <v>3.2114959011475244</v>
+        <v>0.4461100697517395</v>
       </c>
       <c r="J24" s="17" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.2">

</xml_diff>